<commit_message>
Added final grade view
</commit_message>
<xml_diff>
--- a/app/templates/test1.xlsx
+++ b/app/templates/test1.xlsx
@@ -507,12 +507,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>lci2021051</t>
+          <t>LCI2021009</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Shruti Gajbhiye</t>
+          <t>Gaurav Kabra</t>
         </is>
       </c>
       <c r="I2" t="n">
@@ -549,12 +549,12 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>LCI2021009</t>
+          <t>LCI2021001</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Gaurav Kabra</t>
+          <t>Atharv Tiwari</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -591,12 +591,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>LCI2021001</t>
+          <t>LCI2021017</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Atharv Tiwari</t>
+          <t>Prateek Parmar</t>
         </is>
       </c>
       <c r="I4" t="n">
@@ -633,12 +633,12 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>LCI2021017</t>
+          <t>LCI2021024</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Prateek Parmar</t>
+          <t>Rahul Jamwal</t>
         </is>
       </c>
       <c r="I5" t="n">
@@ -675,12 +675,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>LCI2021024</t>
+          <t>LCI2021002</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Rahul Jamwal</t>
+          <t>Harsh Golchha</t>
         </is>
       </c>
       <c r="I6" t="n">
@@ -717,12 +717,12 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>LCI2021002</t>
+          <t>LCI2021007</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Harsh Golchha</t>
+          <t>Sameep Aher</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -759,12 +759,12 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>LCI2021007</t>
+          <t>LCI2021018</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Sameep Aher</t>
+          <t>Vidisha Agarwal</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -801,12 +801,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>LCI2021018</t>
+          <t>LCI2021010</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Vidisha Agarwal</t>
+          <t>Samarth Sharma</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -843,12 +843,12 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>LCI2021010</t>
+          <t>LCI2021057</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Samarth Sharma</t>
+          <t>Rhysha Kachari</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -885,12 +885,12 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>LCI2021057</t>
+          <t>LCI2021011</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Rhysha Kachari</t>
+          <t>Chakradhar Reddy</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -927,12 +927,12 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>LCI2021011</t>
+          <t>LCI2021027</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Chakradhar Reddy</t>
+          <t>Yatharth Jain</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -969,12 +969,12 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>LCI2021027</t>
+          <t>LCI2021035</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Yatharth Jain</t>
+          <t>Saarthak Verma</t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -1011,12 +1011,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>LCI2021035</t>
+          <t>LCI2021043</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Saarthak Verma</t>
+          <t>Bhavya Choudhary</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1053,12 +1053,12 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>LCI2021043</t>
+          <t>LCI2021045</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Bhavya Choudhary</t>
+          <t>Advit Mahale</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1095,12 +1095,12 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>LCI2021045</t>
+          <t>LCI2021051</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Advit Mahale</t>
+          <t>Shruti Gajbhiye</t>
         </is>
       </c>
       <c r="I16" t="n">

</xml_diff>

<commit_message>
View grades functionality added
</commit_message>
<xml_diff>
--- a/app/templates/test1.xlsx
+++ b/app/templates/test1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:H1"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,38 +436,678 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>email</t>
+          <t>year</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>branch</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>subject</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>semester</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>assignment</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>rollno</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>fname</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>lname</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>branch</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>year</t>
-        </is>
-      </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>password</t>
-        </is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>marks</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>max marks</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>CSAI</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>data structures</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>End Semester</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>LCI2021009</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Gaurav Kabra</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>CSAI</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>data structures</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>End Semester</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>LCI2021017</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Prateek Parmar</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>CSAI</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>data structures</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>End Semester</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>LCI2021024</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Rahul Jamwal</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>CSAI</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>data structures</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>End Semester</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>LCI2021002</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Harsh Golchha</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>CSAI</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>data structures</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>End Semester</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>LCI2021007</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Sameep Aher</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>CSAI</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>data structures</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>End Semester</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>LCI2021018</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Vidisha Agarwal</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>CSAI</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>data structures</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>End Semester</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>LCI2021010</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Samarth Sharma</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>CSAI</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>data structures</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>End Semester</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>LCI2021057</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Rhysha Kachari</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>CSAI</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>data structures</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>End Semester</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>LCI2021011</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Chakradhar Reddy</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>CSAI</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>data structures</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>End Semester</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>LCI2021027</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Yatharth Jain</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>CSAI</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>data structures</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>2</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>End Semester</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>LCI2021035</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Saarthak Verma</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>CSAI</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>data structures</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>End Semester</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>LCI2021043</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Bhavya Choudhary</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>CSAI</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>data structures</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>End Semester</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>LCI2021045</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Advit Mahale</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>CSAI</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>data structures</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>2</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>End Semester</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>LCI2021051</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Shruti Gajbhiye</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>CSAI</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>data structures</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>2</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>End Semester</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>LCI2021001</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Atharv Tiwari</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>